<commit_message>
Map switching combo now takes in three buttons
</commit_message>
<xml_diff>
--- a/mapper/LLOAD Mapping.xlsx
+++ b/mapper/LLOAD Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruno/Documents/workspace/LLOAD/mapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A60AE058-E2D5-524B-9924-D15A0750F26D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF6E55AB-B191-8F44-9DF3-CC06DB2E9BFD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14540" activeTab="1" xr2:uid="{1BE5C46B-17CB-E74B-8684-610FF479D74F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="99">
   <si>
     <t>NeoGeo Buttons</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>1 / Start</t>
+  </si>
+  <si>
+    <t>L + R (8)</t>
   </si>
 </sst>
 </file>
@@ -706,18 +709,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55203FE4-31A6-A647-BB25-C576380D446E}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -912,7 +914,7 @@
         <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
         <v>85</v>
@@ -932,7 +934,7 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
@@ -949,7 +951,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -966,7 +968,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
@@ -980,7 +982,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
@@ -994,7 +996,7 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -1005,6 +1007,11 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1018,7 +1025,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1467,7 +1474,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -2177,12 +2184,6 @@
           </x14:formula1>
           <xm:sqref>C3:C27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F40BB70B-1131-B24C-9DCD-F3E9195796BF}">
-          <x14:formula1>
-            <xm:f>_Config!$D$2:$D$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>D3:D27</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{15A4FF06-71DB-5D46-BF7D-6ED9A4F3685C}">
           <x14:formula1>
             <xm:f>_Config!$E$2:$E$15</xm:f>
@@ -2195,6 +2196,12 @@
           </x14:formula1>
           <xm:sqref>F3:F27</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F40BB70B-1131-B24C-9DCD-F3E9195796BF}">
+          <x14:formula1>
+            <xm:f>_Config!$D$2:$D$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D27</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>